<commit_message>
format lại trang excel
</commit_message>
<xml_diff>
--- a/daily report.xlsx
+++ b/daily report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 bluepink@ckdvietnam.com | www.ckdvietname.com | Hotline: 19007327</t>
   </si>
   <si>
-    <t>Nội dung báo cáo</t>
+    <t>NỘI DUNG BÁO CÁO</t>
   </si>
   <si>
     <t>MSNV</t>
@@ -59,13 +59,19 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -77,23 +83,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -241,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +261,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -441,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -453,31 +464,15 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -506,9 +501,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -517,9 +510,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -530,6 +521,54 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -653,55 +692,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -716,120 +752,126 @@
     <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1118,7 +1160,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>579755</xdr:colOff>
+      <xdr:colOff>541655</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>445135</xdr:rowOff>
     </xdr:to>
@@ -1411,193 +1453,199 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="7.14285714285714" customWidth="1"/>
-    <col min="2" max="2" width="10.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="7.71428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.8571428571429" style="1" customWidth="1"/>
+    <col min="3" max="4" width="32.5714285714286" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="78" customHeight="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" ht="18.75" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" ht="62" customHeight="1" spans="1:4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" ht="42" customHeight="1" spans="1:4">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="10" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" ht="22" customHeight="1" spans="1:4">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="14"/>
+    <row r="5" ht="30" customHeight="1" spans="1:4">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:4">
+      <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="14"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:4">
+      <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="14"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:4">
+      <c r="A8" s="12"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="14"/>
+    <row r="9" ht="30" customHeight="1" spans="1:4">
+      <c r="A9" s="12"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="14"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:4">
+      <c r="A10" s="12"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="14"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:4">
+      <c r="A11" s="12"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1606,6 +1654,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>